<commit_message>
transforming error estimates by category, adding source script
</commit_message>
<xml_diff>
--- a/Data/acc_data_reformatted.xlsx
+++ b/Data/acc_data_reformatted.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joribarley/Documents/GitHub/plasticity/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859DBA54-2A96-9445-8441-4A818C69C8C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07F9172-8A7E-9C47-A54E-180C25B415BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="25960" windowHeight="16440" xr2:uid="{71CED034-CA02-F342-B8AB-E8372AC16A5C}"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="25960" windowHeight="16440" xr2:uid="{71CED034-CA02-F342-B8AB-E8372AC16A5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$379:$AK$396</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$X$1:$X$601</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1908,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD823B55-7788-6E47-847E-5FF5E4B6C294}">
   <dimension ref="A1:AK601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P561" workbookViewId="0">
-      <selection activeCell="X566" sqref="X566:X589"/>
+    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
+      <selection activeCell="F376" sqref="F376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>